<commit_message>
update name folder and code
</commit_message>
<xml_diff>
--- a/Python/Data Analysis/DataCate.xlsx
+++ b/Python/Data Analysis/DataCate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://btmglobal-my.sharepoint.com/personal/trieu_pham_btmglobal_com/Documents/Projects/github/python/python/Data Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D646D69-3A13-4157-BC97-C83BB9060AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2D646D69-3A13-4157-BC97-C83BB9060AD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0B89749-0F3F-47D8-A341-77935F4B75F7}"/>
   <bookViews>
-    <workbookView xWindow="39135" yWindow="510" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30360" yWindow="1560" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1277,13 +1277,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D5532"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>

</xml_diff>